<commit_message>
updated the report and completed all report and code
</commit_message>
<xml_diff>
--- a/Performance Analysis.xlsx
+++ b/Performance Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IIT\2nd Year\Alogrithm\Coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344BC46E-1CE0-4D58-AA62-E1030F679928}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783A2B21-881E-464C-84C1-A748A4DE27CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,24 +26,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
-  <si>
-    <t>Performance Analysis of the Algorithm</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Bridge Input Data</t>
-  </si>
-  <si>
-    <t>T1</t>
-  </si>
-  <si>
-    <t>T2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T3 </t>
-  </si>
-  <si>
-    <t>T</t>
   </si>
   <si>
     <t>Ladder Input Data</t>
@@ -52,14 +37,75 @@
     <t>No of Edges</t>
   </si>
   <si>
-    <t>T_avg</t>
+    <t>Performance Analysis of the Algorithm (Updated input data)</t>
+  </si>
+  <si>
+    <t>Inputs data size</t>
+  </si>
+  <si>
+    <t>Edges</t>
+  </si>
+  <si>
+    <t>Nodes</t>
+  </si>
+  <si>
+    <t>Ratio changes in time</t>
+  </si>
+  <si>
+    <r>
+      <t>Log</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ratio of times</t>
+    </r>
+  </si>
+  <si>
+    <t>Bridge Data Input</t>
+  </si>
+  <si>
+    <t>Ladder Data Input</t>
+  </si>
+  <si>
+    <t>Time Taken to produce the outcome (ms)
+(in nanoseconds)Time spent to produce the outcome
+Time Taken to produce the result in seconds</t>
+  </si>
+  <si>
+    <t>T / ms</t>
+  </si>
+  <si>
+    <t>T1/s</t>
+  </si>
+  <si>
+    <t>T2/s</t>
+  </si>
+  <si>
+    <t>T3/s</t>
+  </si>
+  <si>
+    <t>T_avg/s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,19 +137,158 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -112,7 +297,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -127,6 +312,100 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -160,31 +439,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Performance Analysis - bridge -</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -224,7 +478,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Performance Analysis+Sheet1!$A$1</c:v>
+            <c:v>Number of Edges vs Time taken </c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -248,7 +502,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="exp"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -289,67 +543,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>130</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>258</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>514</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1026</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2050</c:v>
+                  <c:v>2048</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$5:$E$13</c:f>
+              <c:f>Sheet1!$F$5:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>1.6666666666666668E-3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3333333333333333E-3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2E-3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.6666666666666668E-3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6666666666666666E-3</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6666666666666666E-3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1999999999999999E-2</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.1666666666666667E-2</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.9E-2</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -357,11 +611,12 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D2D9-4CD9-AF4E-7DEA31510005}"/>
+              <c16:uniqueId val="{00000000-BDF4-4F03-A0D5-D9D0E5516726}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -370,16 +625,76 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="348899120"/>
-        <c:axId val="348899536"/>
+        <c:axId val="555148223"/>
+        <c:axId val="555148639"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="348899120"/>
+        <c:axId val="555148223"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> of Edges</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -417,7 +732,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348899536"/>
+        <c:crossAx val="555148639"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -425,7 +740,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="348899536"/>
+        <c:axId val="555148639"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -446,6 +761,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time Taken / ms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -477,7 +847,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="348899120"/>
+        <c:crossAx val="555148223"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -587,7 +957,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Performance Analysis - ladder -</c:v>
+            <c:v>Number of Edges vs Time Taken</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -611,7 +981,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
+            <c:trendlineType val="exp"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -652,31 +1022,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>94</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>190</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>382</c:v>
+                  <c:v>384</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>766</c:v>
+                  <c:v>768</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1534</c:v>
+                  <c:v>1536</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3070</c:v>
+                  <c:v>3072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -688,31 +1058,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2E-3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.9999999999999993E-3</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1000000000000001E-2</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5999999999999999E-2</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16700000000000001</c:v>
+                  <c:v>167</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0860000000000001</c:v>
+                  <c:v>1086</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.0289999999999999</c:v>
+                  <c:v>7029</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -720,7 +1090,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-FDC7-468D-BC21-08CDCCC76C65}"/>
+              <c16:uniqueId val="{00000000-A3C0-47FC-86EC-AA310866F991}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -733,16 +1103,71 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="342934720"/>
-        <c:axId val="346801248"/>
+        <c:axId val="2081756784"/>
+        <c:axId val="273292080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="342934720"/>
+        <c:axId val="2081756784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of Edges</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -780,7 +1205,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="346801248"/>
+        <c:crossAx val="273292080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -788,7 +1213,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="346801248"/>
+        <c:axId val="273292080"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -809,6 +1234,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time Taken / s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -840,7 +1320,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342934720"/>
+        <c:crossAx val="2081756784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2013,22 +2493,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>209176</xdr:colOff>
+      <xdr:colOff>313765</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>96371</xdr:rowOff>
+      <xdr:rowOff>171076</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>216647</xdr:colOff>
+      <xdr:colOff>321236</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:rowOff>112806</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5346AF0E-BBE5-417C-A266-B3F1E0F8A278}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5216F8D-99FE-48E2-8D33-634B09E75DC9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2049,22 +2529,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>530412</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>126253</xdr:rowOff>
+      <xdr:colOff>13606</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>88897</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>336176</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>67983</xdr:rowOff>
+      <xdr:colOff>1006929</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{069A3CF7-E3EE-44BF-A6B1-B6F5A656ADE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7E7ED1B-8BDC-4680-865B-077A8496B24A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2350,8 +2830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2373,78 +2853,78 @@
   <sheetData>
     <row r="1" spans="1:13" ht="17" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="I4" s="3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="4">
         <v>1E-3</v>
       </c>
       <c r="C5" s="4">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="D5" s="4">
         <v>2E-3</v>
       </c>
       <c r="E5" s="4">
-        <f>AVERAGE(B5:D5)</f>
-        <v>1.6666666666666668E-3</v>
+        <f t="shared" ref="E5:E13" si="0">AVERAGE(B5:D5)</f>
+        <v>1.3333333333333333E-3</v>
       </c>
       <c r="F5" s="4">
-        <f>ROUND(E5,3)</f>
-        <v>2E-3</v>
+        <f>ROUND(E5,3)*1000</f>
+        <v>1</v>
       </c>
       <c r="H5" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I5" s="4">
         <v>3.0000000000000001E-3</v>
@@ -2456,17 +2936,17 @@
         <v>1E-3</v>
       </c>
       <c r="L5" s="4">
-        <f>AVERAGE(I5:K5)</f>
+        <f t="shared" ref="L5:L13" si="1">AVERAGE(I5:K5)</f>
         <v>2E-3</v>
       </c>
       <c r="M5" s="4">
-        <f>ROUND(L5, 3)</f>
-        <v>2E-3</v>
+        <f>ROUND(L5, 3)*1000</f>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4">
         <v>2E-3</v>
@@ -2478,15 +2958,15 @@
         <v>1E-3</v>
       </c>
       <c r="E6" s="4">
-        <f>AVERAGE(B6:D6)</f>
+        <f t="shared" si="0"/>
         <v>1.3333333333333333E-3</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" ref="F6:F13" si="0">ROUND(E6,3)</f>
-        <v>1E-3</v>
+        <f t="shared" ref="F6:F13" si="2">ROUND(E6,3)*1000</f>
+        <v>1</v>
       </c>
       <c r="H6" s="4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I6" s="4">
         <v>2E-3</v>
@@ -2498,17 +2978,17 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="L6" s="4">
-        <f>AVERAGE(I6:K6)</f>
+        <f t="shared" si="1"/>
         <v>3.3333333333333335E-3</v>
       </c>
       <c r="M6" s="4">
-        <f>ROUND(L6, 3)</f>
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" ref="M6:M13" si="3">ROUND(L6, 3)*1000</f>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B7" s="4">
         <v>1E-3</v>
@@ -2520,15 +3000,15 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E7" s="4">
-        <f>AVERAGE(B7:D7)</f>
-        <v>2E-3</v>
-      </c>
-      <c r="F7" s="4">
         <f t="shared" si="0"/>
         <v>2E-3</v>
       </c>
+      <c r="F7" s="4">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
       <c r="H7" s="4">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="I7" s="4">
         <v>7.0000000000000001E-3</v>
@@ -2540,17 +3020,17 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="L7" s="4">
-        <f>AVERAGE(I7:K7)</f>
+        <f t="shared" si="1"/>
         <v>5.3333333333333332E-3</v>
       </c>
       <c r="M7" s="4">
-        <f>ROUND(L7, 3)</f>
-        <v>5.0000000000000001E-3</v>
+        <f t="shared" si="3"/>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B8" s="4">
         <v>1E-3</v>
@@ -2562,15 +3042,15 @@
         <v>2E-3</v>
       </c>
       <c r="E8" s="4">
-        <f>AVERAGE(B8:D8)</f>
+        <f t="shared" si="0"/>
         <v>1.6666666666666668E-3</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" si="0"/>
-        <v>2E-3</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="H8" s="4">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="I8" s="4">
         <v>8.9999999999999993E-3</v>
@@ -2582,17 +3062,17 @@
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="L8" s="4">
-        <f>AVERAGE(I8:K8)</f>
+        <f t="shared" si="1"/>
         <v>8.6666666666666663E-3</v>
       </c>
       <c r="M8" s="4">
-        <f>ROUND(L8, 3)</f>
-        <v>8.9999999999999993E-3</v>
+        <f t="shared" si="3"/>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B9" s="4">
         <v>2E-3</v>
@@ -2604,15 +3084,15 @@
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="E9" s="4">
-        <f>AVERAGE(B9:D9)</f>
+        <f t="shared" si="0"/>
         <v>2.6666666666666666E-3</v>
       </c>
       <c r="F9" s="4">
-        <f t="shared" si="0"/>
-        <v>3.0000000000000001E-3</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="H9" s="4">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="I9" s="4">
         <v>1.7999999999999999E-2</v>
@@ -2624,17 +3104,17 @@
         <v>0.02</v>
       </c>
       <c r="L9" s="4">
-        <f>AVERAGE(I9:K9)</f>
+        <f t="shared" si="1"/>
         <v>2.0666666666666667E-2</v>
       </c>
       <c r="M9" s="4">
-        <f>ROUND(L9, 3)</f>
-        <v>2.1000000000000001E-2</v>
+        <f t="shared" si="3"/>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B10" s="4">
         <v>3.0000000000000001E-3</v>
@@ -2646,15 +3126,15 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="E10" s="4">
-        <f>AVERAGE(B10:D10)</f>
+        <f t="shared" si="0"/>
         <v>3.6666666666666666E-3</v>
       </c>
       <c r="F10" s="4">
-        <f t="shared" si="0"/>
-        <v>4.0000000000000001E-3</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="H10" s="4">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="I10" s="4">
         <v>4.1000000000000002E-2</v>
@@ -2666,17 +3146,17 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="L10" s="4">
-        <f>AVERAGE(I10:K10)</f>
+        <f t="shared" si="1"/>
         <v>4.5666666666666668E-2</v>
       </c>
       <c r="M10" s="4">
-        <f>ROUND(L10, 3)</f>
-        <v>4.5999999999999999E-2</v>
+        <f t="shared" si="3"/>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B11" s="4">
         <v>1.0999999999999999E-2</v>
@@ -2688,15 +3168,15 @@
         <v>1.2999999999999999E-2</v>
       </c>
       <c r="E11" s="4">
-        <f>AVERAGE(B11:D11)</f>
+        <f t="shared" si="0"/>
         <v>1.1999999999999999E-2</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" si="0"/>
-        <v>1.2E-2</v>
+        <f t="shared" si="2"/>
+        <v>12</v>
       </c>
       <c r="H11" s="4">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="I11" s="4">
         <v>0.16500000000000001</v>
@@ -2708,17 +3188,17 @@
         <v>0.16</v>
       </c>
       <c r="L11" s="4">
-        <f>AVERAGE(I11:K11)</f>
+        <f t="shared" si="1"/>
         <v>0.16700000000000001</v>
       </c>
       <c r="M11" s="4">
-        <f>ROUND(L11, 3)</f>
-        <v>0.16700000000000001</v>
+        <f t="shared" si="3"/>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="B12" s="4">
         <v>1.6E-2</v>
@@ -2730,15 +3210,15 @@
         <v>2.5999999999999999E-2</v>
       </c>
       <c r="E12" s="4">
-        <f>AVERAGE(B12:D12)</f>
+        <f t="shared" si="0"/>
         <v>2.1666666666666667E-2</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" si="0"/>
-        <v>2.1999999999999999E-2</v>
+        <f t="shared" si="2"/>
+        <v>22</v>
       </c>
       <c r="H12" s="4">
-        <v>1534</v>
+        <v>1536</v>
       </c>
       <c r="I12" s="4">
         <v>1.046</v>
@@ -2750,17 +3230,17 @@
         <v>1.083</v>
       </c>
       <c r="L12" s="4">
-        <f>AVERAGE(I12:K12)</f>
+        <f t="shared" si="1"/>
         <v>1.0856666666666666</v>
       </c>
       <c r="M12" s="4">
-        <f>ROUND(L12, 3)</f>
-        <v>1.0860000000000001</v>
+        <f t="shared" si="3"/>
+        <v>1086</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
-        <v>2050</v>
+        <v>2048</v>
       </c>
       <c r="B13" s="4">
         <v>4.2999999999999997E-2</v>
@@ -2772,15 +3252,15 @@
         <v>3.5999999999999997E-2</v>
       </c>
       <c r="E13" s="4">
-        <f>AVERAGE(B13:D13)</f>
-        <v>3.9E-2</v>
-      </c>
-      <c r="F13" s="4">
         <f t="shared" si="0"/>
         <v>3.9E-2</v>
       </c>
+      <c r="F13" s="4">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
       <c r="H13" s="4">
-        <v>3070</v>
+        <v>3072</v>
       </c>
       <c r="I13" s="4">
         <v>6.9370000000000003</v>
@@ -2792,12 +3272,12 @@
         <v>7.1070000000000002</v>
       </c>
       <c r="L13" s="4">
-        <f>AVERAGE(I13:K13)</f>
+        <f t="shared" si="1"/>
         <v>7.0289999999999999</v>
       </c>
       <c r="M13" s="4">
-        <f>ROUND(L13, 3)</f>
-        <v>7.0289999999999999</v>
+        <f t="shared" si="3"/>
+        <v>7029</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
@@ -2817,10 +3297,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA9DFDC-8830-4061-9CB4-01445344EC48}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="F4:Z21"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="108" workbookViewId="0">
-      <selection activeCell="G13" sqref="A3:G13"/>
+    <sheetView topLeftCell="E1" zoomScale="86" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2830,24 +3310,558 @@
     <col min="3" max="3" width="9.6328125" customWidth="1"/>
     <col min="4" max="4" width="11.1796875" customWidth="1"/>
     <col min="5" max="5" width="14.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="9" max="9" width="14.6328125" customWidth="1"/>
+    <col min="10" max="10" width="5.90625" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.36328125" customWidth="1"/>
+    <col min="13" max="13" width="0.36328125" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="7.1796875" customWidth="1"/>
+    <col min="21" max="21" width="2.54296875" customWidth="1"/>
+    <col min="24" max="24" width="0.90625" customWidth="1"/>
+    <col min="26" max="26" width="6.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.4">
-      <c r="A1" s="2" t="s">
+    <row r="4" spans="6:26" ht="13" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="6:26" x14ac:dyDescent="0.35">
+      <c r="F8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="6:26" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" s="17"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="18"/>
+      <c r="Q9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="R9" s="9"/>
+      <c r="S9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="T9" s="11"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="W9" s="17"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z9" s="18"/>
+    </row>
+    <row r="10" spans="6:26" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="21"/>
+      <c r="Q10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="S10" s="38"/>
+      <c r="T10" s="39"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="19"/>
+      <c r="W10" s="20"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="21"/>
+    </row>
+    <row r="11" spans="6:26" x14ac:dyDescent="0.35">
+      <c r="F11" s="25">
+        <v>6</v>
+      </c>
+      <c r="G11" s="24">
+        <v>8</v>
+      </c>
+      <c r="H11" s="30">
+        <v>1</v>
+      </c>
+      <c r="I11" s="23"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="30"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="30"/>
+      <c r="O11" s="31"/>
+      <c r="Q11" s="25">
+        <v>6</v>
+      </c>
+      <c r="R11" s="24">
+        <v>12</v>
+      </c>
+      <c r="S11" s="30">
+        <v>2</v>
+      </c>
+      <c r="T11" s="23"/>
+      <c r="U11" s="31"/>
+      <c r="V11" s="23"/>
+      <c r="W11" s="23"/>
+      <c r="X11" s="31"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="31"/>
+    </row>
+    <row r="12" spans="6:26" x14ac:dyDescent="0.35">
+      <c r="F12" s="26">
+        <v>10</v>
+      </c>
+      <c r="G12" s="28">
+        <v>16</v>
+      </c>
+      <c r="H12" s="32">
+        <v>1</v>
+      </c>
+      <c r="I12" s="33"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="32">
+        <v>1</v>
+      </c>
+      <c r="L12" s="33"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="32">
+        <f>ROUND(LOG(K12,2), 3)</f>
         <v>0</v>
       </c>
+      <c r="O12" s="34"/>
+      <c r="Q12" s="26">
+        <v>12</v>
+      </c>
+      <c r="R12" s="28">
+        <v>24</v>
+      </c>
+      <c r="S12" s="32">
+        <v>3</v>
+      </c>
+      <c r="T12" s="33"/>
+      <c r="U12" s="34"/>
+      <c r="V12" s="33">
+        <v>1.5</v>
+      </c>
+      <c r="W12" s="33"/>
+      <c r="X12" s="34"/>
+      <c r="Y12" s="32">
+        <f>ROUND(LOG(V12,2), 3)</f>
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="Z12" s="34"/>
     </row>
-    <row r="4" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+    <row r="13" spans="6:26" x14ac:dyDescent="0.35">
+      <c r="F13" s="26">
+        <v>18</v>
+      </c>
+      <c r="G13" s="28">
+        <v>32</v>
+      </c>
+      <c r="H13" s="32">
+        <v>2</v>
+      </c>
+      <c r="I13" s="33"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="32">
+        <v>2</v>
+      </c>
+      <c r="L13" s="33"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="32">
+        <f t="shared" ref="N13:N19" si="0">ROUND(LOG(K13,2), 3)</f>
+        <v>1</v>
+      </c>
+      <c r="O13" s="34"/>
+      <c r="Q13" s="26">
+        <v>24</v>
+      </c>
+      <c r="R13" s="28">
+        <v>48</v>
+      </c>
+      <c r="S13" s="32">
+        <v>5</v>
+      </c>
+      <c r="T13" s="33"/>
+      <c r="U13" s="34"/>
+      <c r="V13" s="33">
+        <v>1.667</v>
+      </c>
+      <c r="W13" s="33"/>
+      <c r="X13" s="34"/>
+      <c r="Y13" s="32">
+        <f t="shared" ref="Y13:Y19" si="1">ROUND(LOG(V13,2), 3)</f>
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="Z13" s="34"/>
+    </row>
+    <row r="14" spans="6:26" x14ac:dyDescent="0.35">
+      <c r="F14" s="26">
+        <v>34</v>
+      </c>
+      <c r="G14" s="28">
+        <v>64</v>
+      </c>
+      <c r="H14" s="32">
+        <v>2</v>
+      </c>
+      <c r="I14" s="33"/>
+      <c r="J14" s="34"/>
+      <c r="K14" s="32">
+        <v>1</v>
+      </c>
+      <c r="L14" s="33"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="34"/>
+      <c r="Q14" s="26">
+        <v>48</v>
+      </c>
+      <c r="R14" s="28">
+        <v>96</v>
+      </c>
+      <c r="S14" s="32">
+        <v>9</v>
+      </c>
+      <c r="T14" s="33"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="33">
+        <v>1.8</v>
+      </c>
+      <c r="W14" s="33"/>
+      <c r="X14" s="34"/>
+      <c r="Y14" s="32">
+        <f t="shared" si="1"/>
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="Z14" s="34"/>
+    </row>
+    <row r="15" spans="6:26" x14ac:dyDescent="0.35">
+      <c r="F15" s="26">
+        <v>66</v>
+      </c>
+      <c r="G15" s="28">
+        <v>128</v>
+      </c>
+      <c r="H15" s="32">
+        <v>3</v>
+      </c>
+      <c r="I15" s="33"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="32">
+        <v>1.5</v>
+      </c>
+      <c r="L15" s="33"/>
+      <c r="M15" s="34"/>
+      <c r="N15" s="32">
+        <f t="shared" si="0"/>
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="O15" s="34"/>
+      <c r="Q15" s="26">
+        <v>96</v>
+      </c>
+      <c r="R15" s="28">
+        <v>192</v>
+      </c>
+      <c r="S15" s="32">
+        <v>21</v>
+      </c>
+      <c r="T15" s="33"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="33">
+        <v>2.3330000000000002</v>
+      </c>
+      <c r="W15" s="33"/>
+      <c r="X15" s="34"/>
+      <c r="Y15" s="32">
+        <f t="shared" si="1"/>
+        <v>1.222</v>
+      </c>
+      <c r="Z15" s="34"/>
+    </row>
+    <row r="16" spans="6:26" x14ac:dyDescent="0.35">
+      <c r="F16" s="26">
+        <v>130</v>
+      </c>
+      <c r="G16" s="28">
+        <v>256</v>
+      </c>
+      <c r="H16" s="32">
+        <v>4</v>
+      </c>
+      <c r="I16" s="33"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="32">
+        <v>1.333</v>
+      </c>
+      <c r="L16" s="33"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="32">
+        <f t="shared" si="0"/>
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="O16" s="34"/>
+      <c r="Q16" s="26">
+        <v>192</v>
+      </c>
+      <c r="R16" s="28">
+        <v>384</v>
+      </c>
+      <c r="S16" s="32">
+        <v>46</v>
+      </c>
+      <c r="T16" s="33"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="33">
+        <v>2.19</v>
+      </c>
+      <c r="W16" s="33"/>
+      <c r="X16" s="34"/>
+      <c r="Y16" s="32">
+        <f t="shared" si="1"/>
+        <v>1.131</v>
+      </c>
+      <c r="Z16" s="34"/>
+    </row>
+    <row r="17" spans="6:26" x14ac:dyDescent="0.35">
+      <c r="F17" s="26">
+        <v>258</v>
+      </c>
+      <c r="G17" s="28">
+        <v>512</v>
+      </c>
+      <c r="H17" s="32">
+        <v>12</v>
+      </c>
+      <c r="I17" s="33"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="32">
+        <v>3</v>
+      </c>
+      <c r="L17" s="33"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="32">
+        <f t="shared" si="0"/>
+        <v>1.585</v>
+      </c>
+      <c r="O17" s="34"/>
+      <c r="Q17" s="26">
+        <v>384</v>
+      </c>
+      <c r="R17" s="28">
+        <v>768</v>
+      </c>
+      <c r="S17" s="32">
+        <v>167</v>
+      </c>
+      <c r="T17" s="33"/>
+      <c r="U17" s="34"/>
+      <c r="V17" s="33">
+        <v>3.63</v>
+      </c>
+      <c r="W17" s="33"/>
+      <c r="X17" s="34"/>
+      <c r="Y17" s="32">
+        <f t="shared" si="1"/>
+        <v>1.86</v>
+      </c>
+      <c r="Z17" s="34"/>
+    </row>
+    <row r="18" spans="6:26" x14ac:dyDescent="0.35">
+      <c r="F18" s="26">
+        <v>514</v>
+      </c>
+      <c r="G18" s="28">
+        <v>1024</v>
+      </c>
+      <c r="H18" s="32">
+        <v>22</v>
+      </c>
+      <c r="I18" s="33"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="32">
+        <v>1.833</v>
+      </c>
+      <c r="L18" s="33"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="32">
+        <f t="shared" si="0"/>
+        <v>0.874</v>
+      </c>
+      <c r="O18" s="34"/>
+      <c r="Q18" s="26">
+        <v>768</v>
+      </c>
+      <c r="R18" s="28">
+        <v>1536</v>
+      </c>
+      <c r="S18" s="32">
+        <v>1086</v>
+      </c>
+      <c r="T18" s="33"/>
+      <c r="U18" s="34"/>
+      <c r="V18" s="33">
+        <v>6.5030000000000001</v>
+      </c>
+      <c r="W18" s="33"/>
+      <c r="X18" s="34"/>
+      <c r="Y18" s="32">
+        <f t="shared" si="1"/>
+        <v>2.7010000000000001</v>
+      </c>
+      <c r="Z18" s="34"/>
+    </row>
+    <row r="19" spans="6:26" x14ac:dyDescent="0.35">
+      <c r="F19" s="27">
+        <v>1026</v>
+      </c>
+      <c r="G19" s="29">
+        <v>2048</v>
+      </c>
+      <c r="H19" s="35">
+        <v>39</v>
+      </c>
+      <c r="I19" s="36"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="35">
+        <v>1.7729999999999999</v>
+      </c>
+      <c r="L19" s="36"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="35">
+        <f t="shared" si="0"/>
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="O19" s="37"/>
+      <c r="Q19" s="27">
+        <v>1536</v>
+      </c>
+      <c r="R19" s="29">
+        <v>3072</v>
+      </c>
+      <c r="S19" s="35">
+        <v>7029</v>
+      </c>
+      <c r="T19" s="36"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="36">
+        <v>6.4720000000000004</v>
+      </c>
+      <c r="W19" s="36"/>
+      <c r="X19" s="37"/>
+      <c r="Y19" s="35">
+        <f t="shared" si="1"/>
+        <v>2.694</v>
+      </c>
+      <c r="Z19" s="37"/>
+    </row>
+    <row r="20" spans="6:26" x14ac:dyDescent="0.35">
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+    </row>
+    <row r="21" spans="6:26" x14ac:dyDescent="0.35">
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="62">
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="V16:X16"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="S19:U19"/>
+    <mergeCell ref="V11:X11"/>
+    <mergeCell ref="V12:X12"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="V14:X14"/>
+    <mergeCell ref="V17:X17"/>
+    <mergeCell ref="V19:X19"/>
+    <mergeCell ref="V18:X18"/>
+    <mergeCell ref="N17:O17"/>
+    <mergeCell ref="N18:O18"/>
+    <mergeCell ref="N19:O19"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="S17:U17"/>
+    <mergeCell ref="N11:O11"/>
+    <mergeCell ref="N12:O12"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="S9:U10"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:J10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated new times and got 2 as the time complexity
</commit_message>
<xml_diff>
--- a/Performance Analysis.xlsx
+++ b/Performance Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IIT\2nd Year\Alogrithm\Coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{783A2B21-881E-464C-84C1-A748A4DE27CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8C0183A-EE84-4361-AFE3-52FC4D4C7785}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -316,46 +316,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -374,16 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -392,11 +347,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -405,6 +381,30 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -582,28 +582,28 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22</c:v>
+                  <c:v>739</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>39</c:v>
+                  <c:v>3764</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -616,7 +616,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1058,31 +1057,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46</c:v>
+                  <c:v>265</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>167</c:v>
+                  <c:v>625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1086</c:v>
+                  <c:v>3013</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7029</c:v>
+                  <c:v>11935</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2830,8 +2829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="81" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2927,21 +2926,21 @@
         <v>12</v>
       </c>
       <c r="I5" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="J5" s="4">
-        <v>2E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="K5" s="4">
         <v>1E-3</v>
       </c>
       <c r="L5" s="4">
         <f t="shared" ref="L5:L13" si="1">AVERAGE(I5:K5)</f>
-        <v>2E-3</v>
+        <v>6.6666666666666664E-4</v>
       </c>
       <c r="M5" s="4">
         <f>ROUND(L5, 3)*1000</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.35">
@@ -2949,41 +2948,41 @@
         <v>16</v>
       </c>
       <c r="B6" s="4">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="C6" s="4">
-        <v>1E-3</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D6" s="4">
-        <v>1E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>1.3333333333333333E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" ref="F6:F13" si="2">ROUND(E6,3)*1000</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H6" s="4">
         <v>24</v>
       </c>
       <c r="I6" s="4">
-        <v>2E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="J6" s="4">
-        <v>4.0000000000000001E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="K6" s="4">
-        <v>4.0000000000000001E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="L6" s="4">
         <f t="shared" si="1"/>
-        <v>3.3333333333333335E-3</v>
+        <v>1.5666666666666666E-2</v>
       </c>
       <c r="M6" s="4">
         <f t="shared" ref="M6:M13" si="3">ROUND(L6, 3)*1000</f>
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -2991,41 +2990,41 @@
         <v>32</v>
       </c>
       <c r="B7" s="4">
-        <v>1E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C7" s="4">
-        <v>2E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="D7" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>2E-3</v>
+        <v>8.3333333333333332E-3</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H7" s="4">
         <v>48</v>
       </c>
       <c r="I7" s="4">
-        <v>7.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="J7" s="4">
-        <v>5.0000000000000001E-3</v>
+        <v>0.01</v>
       </c>
       <c r="K7" s="4">
-        <v>4.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="L7" s="4">
         <f t="shared" si="1"/>
-        <v>5.3333333333333332E-3</v>
+        <v>1.1666666666666667E-2</v>
       </c>
       <c r="M7" s="4">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -3033,41 +3032,41 @@
         <v>64</v>
       </c>
       <c r="B8" s="4">
-        <v>1E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="C8" s="4">
-        <v>2E-3</v>
+        <v>0.01</v>
       </c>
       <c r="D8" s="4">
-        <v>2E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>1.6666666666666668E-3</v>
+        <v>1.3666666666666667E-2</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="H8" s="4">
         <v>96</v>
       </c>
       <c r="I8" s="4">
-        <v>8.9999999999999993E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="J8" s="4">
-        <v>0.01</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K8" s="4">
-        <v>7.0000000000000001E-3</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="L8" s="4">
         <f t="shared" si="1"/>
-        <v>8.6666666666666663E-3</v>
+        <v>2.2333333333333334E-2</v>
       </c>
       <c r="M8" s="4">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -3075,41 +3074,41 @@
         <v>128</v>
       </c>
       <c r="B9" s="4">
-        <v>2E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C9" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D9" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>2.6666666666666666E-3</v>
+        <v>1.5333333333333332E-2</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="H9" s="4">
         <v>192</v>
       </c>
       <c r="I9" s="4">
-        <v>1.7999999999999999E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="J9" s="4">
-        <v>2.4E-2</v>
+        <v>6.0999999999999999E-2</v>
       </c>
       <c r="K9" s="4">
-        <v>0.02</v>
+        <v>6.2E-2</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" si="1"/>
-        <v>2.0666666666666667E-2</v>
+        <v>5.7999999999999996E-2</v>
       </c>
       <c r="M9" s="4">
         <f t="shared" si="3"/>
-        <v>21</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.35">
@@ -3117,41 +3116,41 @@
         <v>256</v>
       </c>
       <c r="B10" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>6.3E-2</v>
       </c>
       <c r="C10" s="4">
-        <v>3.0000000000000001E-3</v>
+        <v>0.08</v>
       </c>
       <c r="D10" s="4">
-        <v>5.0000000000000001E-3</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>3.6666666666666666E-3</v>
+        <v>7.0333333333333345E-2</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="H10" s="4">
         <v>384</v>
       </c>
       <c r="I10" s="4">
-        <v>4.1000000000000002E-2</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="J10" s="4">
-        <v>5.0999999999999997E-2</v>
+        <v>0.12</v>
       </c>
       <c r="K10" s="4">
-        <v>4.4999999999999998E-2</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="L10" s="4">
         <f t="shared" si="1"/>
-        <v>4.5666666666666668E-2</v>
+        <v>0.26466666666666666</v>
       </c>
       <c r="M10" s="4">
         <f t="shared" si="3"/>
-        <v>46</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.35">
@@ -3159,41 +3158,41 @@
         <v>512</v>
       </c>
       <c r="B11" s="4">
-        <v>1.0999999999999999E-2</v>
+        <v>0.188</v>
       </c>
       <c r="C11" s="4">
-        <v>1.2E-2</v>
+        <v>0.187</v>
       </c>
       <c r="D11" s="4">
-        <v>1.2999999999999999E-2</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>1.1999999999999999E-2</v>
+        <v>0.19000000000000003</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>190</v>
       </c>
       <c r="H11" s="4">
         <v>768</v>
       </c>
       <c r="I11" s="4">
-        <v>0.16500000000000001</v>
+        <v>0.68500000000000005</v>
       </c>
       <c r="J11" s="4">
-        <v>0.17599999999999999</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="K11" s="4">
-        <v>0.16</v>
+        <v>0.71599999999999997</v>
       </c>
       <c r="L11" s="4">
         <f t="shared" si="1"/>
-        <v>0.16700000000000001</v>
+        <v>0.62466666666666659</v>
       </c>
       <c r="M11" s="4">
         <f t="shared" si="3"/>
-        <v>167</v>
+        <v>625</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
@@ -3201,41 +3200,41 @@
         <v>1024</v>
       </c>
       <c r="B12" s="4">
-        <v>1.6E-2</v>
+        <v>0.62</v>
       </c>
       <c r="C12" s="4">
-        <v>2.3E-2</v>
+        <v>0.56599999999999995</v>
       </c>
       <c r="D12" s="4">
-        <v>2.5999999999999999E-2</v>
+        <v>1.032</v>
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>2.1666666666666667E-2</v>
+        <v>0.73933333333333329</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>739</v>
       </c>
       <c r="H12" s="4">
         <v>1536</v>
       </c>
       <c r="I12" s="4">
-        <v>1.046</v>
+        <v>2.758</v>
       </c>
       <c r="J12" s="4">
-        <v>1.1279999999999999</v>
+        <v>2.948</v>
       </c>
       <c r="K12" s="4">
-        <v>1.083</v>
+        <v>3.3330000000000002</v>
       </c>
       <c r="L12" s="4">
         <f t="shared" si="1"/>
-        <v>1.0856666666666666</v>
+        <v>3.0129999999999999</v>
       </c>
       <c r="M12" s="4">
         <f t="shared" si="3"/>
-        <v>1086</v>
+        <v>3013</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -3243,41 +3242,41 @@
         <v>2048</v>
       </c>
       <c r="B13" s="4">
-        <v>4.2999999999999997E-2</v>
+        <v>3.2130000000000001</v>
       </c>
       <c r="C13" s="4">
-        <v>3.7999999999999999E-2</v>
+        <v>4.2229999999999999</v>
       </c>
       <c r="D13" s="4">
-        <v>3.5999999999999997E-2</v>
+        <v>3.855</v>
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>3.9E-2</v>
+        <v>3.7636666666666669</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>3764</v>
       </c>
       <c r="H13" s="4">
         <v>3072</v>
       </c>
       <c r="I13" s="4">
-        <v>6.9370000000000003</v>
+        <v>11.457000000000001</v>
       </c>
       <c r="J13" s="4">
-        <v>7.0430000000000001</v>
+        <v>11.64</v>
       </c>
       <c r="K13" s="4">
-        <v>7.1070000000000002</v>
+        <v>12.707000000000001</v>
       </c>
       <c r="L13" s="4">
         <f t="shared" si="1"/>
-        <v>7.0289999999999999</v>
+        <v>11.934666666666667</v>
       </c>
       <c r="M13" s="4">
         <f t="shared" si="3"/>
-        <v>7029</v>
+        <v>11935</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
@@ -3299,8 +3298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA9DFDC-8830-4061-9CB4-01445344EC48}">
   <dimension ref="F4:Z21"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="86" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="AB13" sqref="AB13"/>
+    <sheetView topLeftCell="N6" zoomScale="139" zoomScaleNormal="112" workbookViewId="0">
+      <selection activeCell="AB12" sqref="AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3331,42 +3330,42 @@
       </c>
     </row>
     <row r="9" spans="6:26" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="10" t="s">
+      <c r="G9" s="37"/>
+      <c r="H9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="16" t="s">
+      <c r="I9" s="28"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="L9" s="17"/>
-      <c r="M9" s="18"/>
-      <c r="N9" s="16" t="s">
+      <c r="L9" s="34"/>
+      <c r="M9" s="35"/>
+      <c r="N9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="18"/>
-      <c r="Q9" s="8" t="s">
+      <c r="O9" s="35"/>
+      <c r="Q9" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="R9" s="9"/>
-      <c r="S9" s="10" t="s">
+      <c r="R9" s="37"/>
+      <c r="S9" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="T9" s="11"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="16" t="s">
+      <c r="T9" s="28"/>
+      <c r="U9" s="29"/>
+      <c r="V9" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="W9" s="17"/>
-      <c r="X9" s="18"/>
-      <c r="Y9" s="16" t="s">
+      <c r="W9" s="34"/>
+      <c r="X9" s="35"/>
+      <c r="Y9" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="Z9" s="18"/>
+      <c r="Z9" s="35"/>
     </row>
     <row r="10" spans="6:26" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F10" s="7" t="s">
@@ -3375,414 +3374,414 @@
       <c r="G10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="21"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="21"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="10"/>
       <c r="Q10" s="7" t="s">
         <v>6</v>
       </c>
       <c r="R10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="S10" s="38"/>
-      <c r="T10" s="39"/>
-      <c r="U10" s="40"/>
-      <c r="V10" s="19"/>
-      <c r="W10" s="20"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="22"/>
-      <c r="Z10" s="21"/>
+      <c r="S10" s="30"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="11"/>
+      <c r="Z10" s="10"/>
     </row>
     <row r="11" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F11" s="25">
+      <c r="F11" s="13">
         <v>6</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="12">
         <v>8</v>
       </c>
-      <c r="H11" s="30">
+      <c r="H11" s="23">
         <v>1</v>
       </c>
-      <c r="I11" s="23"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="30"/>
-      <c r="O11" s="31"/>
-      <c r="Q11" s="25">
+      <c r="I11" s="26"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="24"/>
+      <c r="Q11" s="13">
         <v>6</v>
       </c>
-      <c r="R11" s="24">
+      <c r="R11" s="12">
         <v>12</v>
       </c>
-      <c r="S11" s="30">
-        <v>2</v>
-      </c>
-      <c r="T11" s="23"/>
-      <c r="U11" s="31"/>
-      <c r="V11" s="23"/>
-      <c r="W11" s="23"/>
-      <c r="X11" s="31"/>
-      <c r="Y11" s="30"/>
-      <c r="Z11" s="31"/>
+      <c r="S11" s="23">
+        <v>1</v>
+      </c>
+      <c r="T11" s="26"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="26"/>
+      <c r="W11" s="26"/>
+      <c r="X11" s="24"/>
+      <c r="Y11" s="23"/>
+      <c r="Z11" s="24"/>
     </row>
     <row r="12" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F12" s="26">
+      <c r="F12" s="14">
         <v>10</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="16">
         <v>16</v>
       </c>
-      <c r="H12" s="32">
-        <v>1</v>
-      </c>
-      <c r="I12" s="33"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="32">
-        <v>1</v>
-      </c>
-      <c r="L12" s="33"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="32">
+      <c r="H12" s="18">
+        <v>4</v>
+      </c>
+      <c r="I12" s="22"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="18">
+        <v>4</v>
+      </c>
+      <c r="L12" s="22"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="18">
         <f>ROUND(LOG(K12,2), 3)</f>
-        <v>0</v>
-      </c>
-      <c r="O12" s="34"/>
-      <c r="Q12" s="26">
+        <v>2</v>
+      </c>
+      <c r="O12" s="19"/>
+      <c r="Q12" s="14">
         <v>12</v>
       </c>
-      <c r="R12" s="28">
+      <c r="R12" s="16">
         <v>24</v>
       </c>
-      <c r="S12" s="32">
-        <v>3</v>
-      </c>
-      <c r="T12" s="33"/>
-      <c r="U12" s="34"/>
-      <c r="V12" s="33">
-        <v>1.5</v>
-      </c>
-      <c r="W12" s="33"/>
-      <c r="X12" s="34"/>
-      <c r="Y12" s="32">
+      <c r="S12" s="18">
+        <v>16</v>
+      </c>
+      <c r="T12" s="22"/>
+      <c r="U12" s="19"/>
+      <c r="V12" s="22">
+        <v>16</v>
+      </c>
+      <c r="W12" s="22"/>
+      <c r="X12" s="19"/>
+      <c r="Y12" s="18">
         <f>ROUND(LOG(V12,2), 3)</f>
-        <v>0.58499999999999996</v>
-      </c>
-      <c r="Z12" s="34"/>
+        <v>4</v>
+      </c>
+      <c r="Z12" s="19"/>
     </row>
     <row r="13" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F13" s="26">
+      <c r="F13" s="14">
         <v>18</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="16">
         <v>32</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="18">
+        <v>8</v>
+      </c>
+      <c r="I13" s="22"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="18">
         <v>2</v>
       </c>
-      <c r="I13" s="33"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="32">
-        <v>2</v>
-      </c>
-      <c r="L13" s="33"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="32">
+      <c r="L13" s="22"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="18">
         <f t="shared" ref="N13:N19" si="0">ROUND(LOG(K13,2), 3)</f>
         <v>1</v>
       </c>
-      <c r="O13" s="34"/>
-      <c r="Q13" s="26">
+      <c r="O13" s="19"/>
+      <c r="Q13" s="14">
         <v>24</v>
       </c>
-      <c r="R13" s="28">
+      <c r="R13" s="16">
         <v>48</v>
       </c>
-      <c r="S13" s="32">
-        <v>5</v>
-      </c>
-      <c r="T13" s="33"/>
-      <c r="U13" s="34"/>
-      <c r="V13" s="33">
-        <v>1.667</v>
-      </c>
-      <c r="W13" s="33"/>
-      <c r="X13" s="34"/>
-      <c r="Y13" s="32">
+      <c r="S13" s="18">
+        <v>12</v>
+      </c>
+      <c r="T13" s="22"/>
+      <c r="U13" s="19"/>
+      <c r="V13" s="22">
+        <v>0.75</v>
+      </c>
+      <c r="W13" s="22"/>
+      <c r="X13" s="19"/>
+      <c r="Y13" s="18">
         <f t="shared" ref="Y13:Y19" si="1">ROUND(LOG(V13,2), 3)</f>
-        <v>0.73699999999999999</v>
-      </c>
-      <c r="Z13" s="34"/>
+        <v>-0.41499999999999998</v>
+      </c>
+      <c r="Z13" s="19"/>
     </row>
     <row r="14" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F14" s="26">
+      <c r="F14" s="14">
         <v>34</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="16">
         <v>64</v>
       </c>
-      <c r="H14" s="32">
-        <v>2</v>
-      </c>
-      <c r="I14" s="33"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="32">
-        <v>1</v>
-      </c>
-      <c r="L14" s="33"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="32">
+      <c r="H14" s="18">
+        <v>14</v>
+      </c>
+      <c r="I14" s="22"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="18">
+        <v>1.75</v>
+      </c>
+      <c r="L14" s="22"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="34"/>
-      <c r="Q14" s="26">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="O14" s="19"/>
+      <c r="Q14" s="14">
         <v>48</v>
       </c>
-      <c r="R14" s="28">
+      <c r="R14" s="16">
         <v>96</v>
       </c>
-      <c r="S14" s="32">
-        <v>9</v>
-      </c>
-      <c r="T14" s="33"/>
-      <c r="U14" s="34"/>
-      <c r="V14" s="33">
-        <v>1.8</v>
-      </c>
-      <c r="W14" s="33"/>
-      <c r="X14" s="34"/>
-      <c r="Y14" s="32">
+      <c r="S14" s="18">
+        <v>22</v>
+      </c>
+      <c r="T14" s="22"/>
+      <c r="U14" s="19"/>
+      <c r="V14" s="22">
+        <v>1.833</v>
+      </c>
+      <c r="W14" s="22"/>
+      <c r="X14" s="19"/>
+      <c r="Y14" s="18">
         <f t="shared" si="1"/>
-        <v>0.84799999999999998</v>
-      </c>
-      <c r="Z14" s="34"/>
+        <v>0.874</v>
+      </c>
+      <c r="Z14" s="19"/>
     </row>
     <row r="15" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F15" s="26">
+      <c r="F15" s="14">
         <v>66</v>
       </c>
-      <c r="G15" s="28">
+      <c r="G15" s="16">
         <v>128</v>
       </c>
-      <c r="H15" s="32">
-        <v>3</v>
-      </c>
-      <c r="I15" s="33"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="32">
-        <v>1.5</v>
-      </c>
-      <c r="L15" s="33"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="32">
+      <c r="H15" s="18">
+        <v>15</v>
+      </c>
+      <c r="I15" s="22"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="18">
+        <v>1.071</v>
+      </c>
+      <c r="L15" s="22"/>
+      <c r="M15" s="19"/>
+      <c r="N15" s="18">
         <f t="shared" si="0"/>
-        <v>0.58499999999999996</v>
-      </c>
-      <c r="O15" s="34"/>
-      <c r="Q15" s="26">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="O15" s="19"/>
+      <c r="Q15" s="14">
         <v>96</v>
       </c>
-      <c r="R15" s="28">
+      <c r="R15" s="16">
         <v>192</v>
       </c>
-      <c r="S15" s="32">
-        <v>21</v>
-      </c>
-      <c r="T15" s="33"/>
-      <c r="U15" s="34"/>
-      <c r="V15" s="33">
-        <v>2.3330000000000002</v>
-      </c>
-      <c r="W15" s="33"/>
-      <c r="X15" s="34"/>
-      <c r="Y15" s="32">
+      <c r="S15" s="18">
+        <v>58</v>
+      </c>
+      <c r="T15" s="22"/>
+      <c r="U15" s="19"/>
+      <c r="V15" s="22">
+        <v>2.6360000000000001</v>
+      </c>
+      <c r="W15" s="22"/>
+      <c r="X15" s="19"/>
+      <c r="Y15" s="18">
         <f t="shared" si="1"/>
-        <v>1.222</v>
-      </c>
-      <c r="Z15" s="34"/>
+        <v>1.3979999999999999</v>
+      </c>
+      <c r="Z15" s="19"/>
     </row>
     <row r="16" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F16" s="26">
+      <c r="F16" s="14">
         <v>130</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="16">
         <v>256</v>
       </c>
-      <c r="H16" s="32">
-        <v>4</v>
-      </c>
-      <c r="I16" s="33"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="32">
-        <v>1.333</v>
-      </c>
-      <c r="L16" s="33"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="32">
+      <c r="H16" s="18">
+        <v>70</v>
+      </c>
+      <c r="I16" s="22"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="18">
+        <v>4.6669999999999998</v>
+      </c>
+      <c r="L16" s="22"/>
+      <c r="M16" s="19"/>
+      <c r="N16" s="18">
         <f t="shared" si="0"/>
-        <v>0.41499999999999998</v>
-      </c>
-      <c r="O16" s="34"/>
-      <c r="Q16" s="26">
+        <v>2.222</v>
+      </c>
+      <c r="O16" s="19"/>
+      <c r="Q16" s="14">
         <v>192</v>
       </c>
-      <c r="R16" s="28">
+      <c r="R16" s="16">
         <v>384</v>
       </c>
-      <c r="S16" s="32">
-        <v>46</v>
-      </c>
-      <c r="T16" s="33"/>
-      <c r="U16" s="34"/>
-      <c r="V16" s="33">
-        <v>2.19</v>
-      </c>
-      <c r="W16" s="33"/>
-      <c r="X16" s="34"/>
-      <c r="Y16" s="32">
+      <c r="S16" s="18">
+        <v>265</v>
+      </c>
+      <c r="T16" s="22"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="22">
+        <v>4.569</v>
+      </c>
+      <c r="W16" s="22"/>
+      <c r="X16" s="19"/>
+      <c r="Y16" s="18">
         <f t="shared" si="1"/>
-        <v>1.131</v>
-      </c>
-      <c r="Z16" s="34"/>
+        <v>2.1920000000000002</v>
+      </c>
+      <c r="Z16" s="19"/>
     </row>
     <row r="17" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F17" s="26">
+      <c r="F17" s="14">
         <v>258</v>
       </c>
-      <c r="G17" s="28">
+      <c r="G17" s="16">
         <v>512</v>
       </c>
-      <c r="H17" s="32">
-        <v>12</v>
-      </c>
-      <c r="I17" s="33"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="32">
-        <v>3</v>
-      </c>
-      <c r="L17" s="33"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="32">
+      <c r="H17" s="18">
+        <v>190</v>
+      </c>
+      <c r="I17" s="22"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="18">
+        <v>2.714</v>
+      </c>
+      <c r="L17" s="22"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="18">
         <f t="shared" si="0"/>
-        <v>1.585</v>
-      </c>
-      <c r="O17" s="34"/>
-      <c r="Q17" s="26">
+        <v>1.44</v>
+      </c>
+      <c r="O17" s="19"/>
+      <c r="Q17" s="14">
         <v>384</v>
       </c>
-      <c r="R17" s="28">
+      <c r="R17" s="16">
         <v>768</v>
       </c>
-      <c r="S17" s="32">
-        <v>167</v>
-      </c>
-      <c r="T17" s="33"/>
-      <c r="U17" s="34"/>
-      <c r="V17" s="33">
-        <v>3.63</v>
-      </c>
-      <c r="W17" s="33"/>
-      <c r="X17" s="34"/>
-      <c r="Y17" s="32">
+      <c r="S17" s="18">
+        <v>625</v>
+      </c>
+      <c r="T17" s="22"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="22">
+        <v>2.3580000000000001</v>
+      </c>
+      <c r="W17" s="22"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="18">
         <f t="shared" si="1"/>
-        <v>1.86</v>
-      </c>
-      <c r="Z17" s="34"/>
+        <v>1.238</v>
+      </c>
+      <c r="Z17" s="19"/>
     </row>
     <row r="18" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F18" s="26">
+      <c r="F18" s="14">
         <v>514</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="16">
         <v>1024</v>
       </c>
-      <c r="H18" s="32">
-        <v>22</v>
-      </c>
-      <c r="I18" s="33"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="32">
-        <v>1.833</v>
-      </c>
-      <c r="L18" s="33"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="32">
+      <c r="H18" s="18">
+        <v>739</v>
+      </c>
+      <c r="I18" s="22"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="18">
+        <v>3.8889999999999998</v>
+      </c>
+      <c r="L18" s="22"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="18">
         <f t="shared" si="0"/>
-        <v>0.874</v>
-      </c>
-      <c r="O18" s="34"/>
-      <c r="Q18" s="26">
+        <v>1.9590000000000001</v>
+      </c>
+      <c r="O18" s="19"/>
+      <c r="Q18" s="14">
         <v>768</v>
       </c>
-      <c r="R18" s="28">
+      <c r="R18" s="16">
         <v>1536</v>
       </c>
-      <c r="S18" s="32">
-        <v>1086</v>
-      </c>
-      <c r="T18" s="33"/>
-      <c r="U18" s="34"/>
-      <c r="V18" s="33">
-        <v>6.5030000000000001</v>
-      </c>
-      <c r="W18" s="33"/>
-      <c r="X18" s="34"/>
-      <c r="Y18" s="32">
+      <c r="S18" s="18">
+        <v>3013</v>
+      </c>
+      <c r="T18" s="22"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="22">
+        <v>4.8209999999999997</v>
+      </c>
+      <c r="W18" s="22"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="18">
         <f t="shared" si="1"/>
-        <v>2.7010000000000001</v>
-      </c>
-      <c r="Z18" s="34"/>
+        <v>2.2690000000000001</v>
+      </c>
+      <c r="Z18" s="19"/>
     </row>
     <row r="19" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F19" s="27">
+      <c r="F19" s="15">
         <v>1026</v>
       </c>
-      <c r="G19" s="29">
+      <c r="G19" s="17">
         <v>2048</v>
       </c>
-      <c r="H19" s="35">
-        <v>39</v>
-      </c>
-      <c r="I19" s="36"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="35">
-        <v>1.7729999999999999</v>
-      </c>
-      <c r="L19" s="36"/>
-      <c r="M19" s="37"/>
-      <c r="N19" s="35">
+      <c r="H19" s="20">
+        <v>3764</v>
+      </c>
+      <c r="I19" s="25"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="20">
+        <v>5.093</v>
+      </c>
+      <c r="L19" s="25"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="20">
         <f t="shared" si="0"/>
-        <v>0.82599999999999996</v>
-      </c>
-      <c r="O19" s="37"/>
-      <c r="Q19" s="27">
+        <v>2.3490000000000002</v>
+      </c>
+      <c r="O19" s="21"/>
+      <c r="Q19" s="15">
         <v>1536</v>
       </c>
-      <c r="R19" s="29">
+      <c r="R19" s="17">
         <v>3072</v>
       </c>
-      <c r="S19" s="35">
-        <v>7029</v>
-      </c>
-      <c r="T19" s="36"/>
-      <c r="U19" s="37"/>
-      <c r="V19" s="36">
-        <v>6.4720000000000004</v>
-      </c>
-      <c r="W19" s="36"/>
-      <c r="X19" s="37"/>
-      <c r="Y19" s="35">
+      <c r="S19" s="20">
+        <v>11935</v>
+      </c>
+      <c r="T19" s="25"/>
+      <c r="U19" s="21"/>
+      <c r="V19" s="25">
+        <v>3.9609999999999999</v>
+      </c>
+      <c r="W19" s="25"/>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="20">
         <f t="shared" si="1"/>
-        <v>2.694</v>
-      </c>
-      <c r="Z19" s="37"/>
+        <v>1.986</v>
+      </c>
+      <c r="Z19" s="21"/>
     </row>
     <row r="20" spans="6:26" x14ac:dyDescent="0.35">
       <c r="F20" s="4"/>
@@ -3798,26 +3797,32 @@
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="V16:X16"/>
-    <mergeCell ref="Y11:Z11"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="S18:U18"/>
-    <mergeCell ref="S19:U19"/>
-    <mergeCell ref="V11:X11"/>
-    <mergeCell ref="V12:X12"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="V15:X15"/>
-    <mergeCell ref="V14:X14"/>
-    <mergeCell ref="V17:X17"/>
-    <mergeCell ref="V19:X19"/>
-    <mergeCell ref="V18:X18"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:J10"/>
+    <mergeCell ref="S9:U10"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="Y9:Z9"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="H12:J12"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="N9:O9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="K16:M16"/>
+    <mergeCell ref="K17:M17"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="H13:J13"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="H15:J15"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="H18:J18"/>
     <mergeCell ref="N17:O17"/>
     <mergeCell ref="N18:O18"/>
     <mergeCell ref="N19:O19"/>
@@ -3834,32 +3839,26 @@
     <mergeCell ref="N14:O14"/>
     <mergeCell ref="N15:O15"/>
     <mergeCell ref="N16:O16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="K16:M16"/>
-    <mergeCell ref="K17:M17"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="H13:J13"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="H15:J15"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="S9:U10"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="Y9:Z9"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="H12:J12"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="N9:O9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="H9:J10"/>
+    <mergeCell ref="S18:U18"/>
+    <mergeCell ref="S19:U19"/>
+    <mergeCell ref="V11:X11"/>
+    <mergeCell ref="V12:X12"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="V14:X14"/>
+    <mergeCell ref="V17:X17"/>
+    <mergeCell ref="V19:X19"/>
+    <mergeCell ref="V18:X18"/>
+    <mergeCell ref="Y11:Z11"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="Y19:Z19"/>
+    <mergeCell ref="V16:X16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>